<commit_message>
Positive test scenario automation script complete for Customer Module
</commit_message>
<xml_diff>
--- a/src/test/java/com/guru99BankingDemo/testData/CustomerModuleData.xlsx
+++ b/src/test/java/com/guru99BankingDemo/testData/CustomerModuleData.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NewCustomerData" sheetId="5" r:id="rId1"/>
-    <sheet name="DeleteCusomerData" sheetId="2" r:id="rId2"/>
+    <sheet name="DeleteCustomerData" sheetId="2" r:id="rId2"/>
     <sheet name="nnn" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:M32"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
   <si>
     <t>Password</t>
   </si>
@@ -103,6 +102,9 @@
   </si>
   <si>
     <t>#$.sdsdds-</t>
+  </si>
+  <si>
+    <t>retfrtfrtr</t>
   </si>
 </sst>
 </file>
@@ -207,13 +209,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -537,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -545,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,46 +569,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="39" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="7"/>
-    </row>
-    <row r="2" spans="1:14" customFormat="1">
+      <c r="M1" s="7"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -621,314 +622,310 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" customFormat="1">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="C3" s="4">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4">
         <v>22</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1998</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>12123</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>1795486253</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14" customFormat="1">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:14">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="C4" s="4">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4">
         <v>22</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>1998</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>1212345</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>1795486253</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" customFormat="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:14">
+      <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="C5" s="4">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
         <v>22</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1998</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>1795486253</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" customFormat="1">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:14">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="C6" s="4">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4">
         <v>22</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1998</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>191212</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:14" customFormat="1">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:14">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="C7" s="4">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4">
         <v>22</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>1998</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>123456</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>191212</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="4">
         <v>1795486253</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" customFormat="1">
-      <c r="A8" s="5">
+    <row r="8" spans="1:14">
+      <c r="A8" s="4">
         <v>522</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="C8" s="4">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4">
         <v>22</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1998</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>191212</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>1795486253</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14" customFormat="1">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="C9" s="4">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4">
         <v>22</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>1998</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>123456</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>191212</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="4">
         <v>1795486253</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:14" customFormat="1">
-      <c r="A10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:14">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="C10" s="4">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4">
         <v>22</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>1998</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>191212</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>1795486253</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:14" customFormat="1"/>
-    <row r="12" spans="1:14" customFormat="1"/>
-    <row r="13" spans="1:14" customFormat="1"/>
-    <row r="14" spans="1:14" customFormat="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1"/>
@@ -947,10 +944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -964,33 +961,29 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="6">
-        <v>20111</v>
+      <c r="A2" s="5">
+        <v>2011</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="6">
-        <v>2011152542</v>
-      </c>
+      <c r="A3" s="5"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="6"/>
+      <c r="A4" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="3"/>
+      <c r="A5" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="56@gmail.com"/>
-    <hyperlink ref="A5" r:id="rId2" display="ewdrfe89798778@.vim"/>
+    <hyperlink ref="A4" r:id="rId1" display="ewdrfe89798778@.vim"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -998,7 +991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1010,40 +1003,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1061,41 +1054,41 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="30">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5">
-        <v>11</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="C3" s="4">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4">
         <v>22</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1998</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>12123</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="4">
         <v>1795486253</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete Customer Module Automation test
</commit_message>
<xml_diff>
--- a/src/test/java/com/guru99BankingDemo/testData/CustomerModuleData.xlsx
+++ b/src/test/java/com/guru99BankingDemo/testData/CustomerModuleData.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="23415" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewCustomerData" sheetId="5" r:id="rId1"/>
-    <sheet name="DeleteCustomerData" sheetId="2" r:id="rId2"/>
-    <sheet name="nnn" sheetId="6" r:id="rId3"/>
+    <sheet name="EditDeleteCustomerIdData" sheetId="2" r:id="rId2"/>
+    <sheet name="EditCustomerData" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="37">
   <si>
     <t>Password</t>
   </si>
@@ -105,6 +105,33 @@
   </si>
   <si>
     <t>retfrtfrtr</t>
+  </si>
+  <si>
+    <t>dfdf</t>
+  </si>
+  <si>
+    <t>dfdfdf</t>
+  </si>
+  <si>
+    <t>sdsds@gmail.com</t>
+  </si>
+  <si>
+    <t>!@#$%^</t>
+  </si>
+  <si>
+    <t>sfdasd</t>
+  </si>
+  <si>
+    <t>dfsgdfgdfgfg</t>
+  </si>
+  <si>
+    <t>!@#$%</t>
+  </si>
+  <si>
+    <t>dfedfdfd</t>
+  </si>
+  <si>
+    <t>!#$%.com</t>
   </si>
 </sst>
 </file>
@@ -161,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -197,6 +224,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -209,7 +249,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -229,6 +269,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -538,7 +584,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,7 +595,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -946,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -989,112 +1035,269 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="32.42578125" customWidth="1"/>
-    <col min="9" max="9" width="36.85546875" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="6" max="6" width="58.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4">
-        <v>22</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1998</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="4">
-        <v>12123</v>
-      </c>
-      <c r="J3" s="4">
-        <v>1795486253</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>17</v>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5">
+        <v>19127</v>
+      </c>
+      <c r="E3" s="9">
+        <v>654685625</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="9">
+        <v>654685625</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="9">
+        <v>654685625</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="5">
+        <v>191275</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="5">
+        <v>191275</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5">
+        <v>454245</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5">
+        <v>191275</v>
+      </c>
+      <c r="E8" s="9">
+        <v>654685625</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="5">
+        <v>191275</v>
+      </c>
+      <c r="E9" s="9">
+        <v>654685625</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="5">
+        <v>45444</v>
+      </c>
+      <c r="D10" s="5">
+        <v>191275</v>
+      </c>
+      <c r="E10" s="9">
+        <v>654685625</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="5">
+        <v>191275</v>
+      </c>
+      <c r="E11" s="9">
+        <v>654685625</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="5">
+        <v>191275</v>
+      </c>
+      <c r="E12" s="9">
+        <v>654685625</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="E7" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="F10" r:id="rId11"/>
+    <hyperlink ref="B10" r:id="rId12" display="!@#$%"/>
+    <hyperlink ref="F11" r:id="rId13"/>
+    <hyperlink ref="B11" r:id="rId14" display="!@#$%"/>
+    <hyperlink ref="F12" r:id="rId15" display="sdsds@gmail.com"/>
+    <hyperlink ref="B12" r:id="rId16" display="!@#$%"/>
+    <hyperlink ref="C11" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>